<commit_message>
Add processed finance and customer data files; update generated customer records
</commit_message>
<xml_diff>
--- a/output/processed_realestate_buyers.xlsx
+++ b/output/processed_realestate_buyers.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aligno\AI Processing\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252DC756-D619-4B41-995D-D4789B340A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49AE3AC-EE21-4C4D-A608-F802669318AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4217,18 +4230,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="27.3984375" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.69921875" customWidth="1"/>
-    <col min="9" max="9" width="16.09765625" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="23.8984375" customWidth="1"/>
+    <col min="5" max="5" width="9.69921875" customWidth="1"/>
+    <col min="6" max="6" width="18.796875" customWidth="1"/>
+    <col min="7" max="7" width="21.69921875" customWidth="1"/>
+    <col min="8" max="8" width="16.8984375" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>